<commit_message>
Updated Control Bit Map
Now contains JR and description of control bits
</commit_message>
<xml_diff>
--- a/Control_Bit_Map.xlsx
+++ b/Control_Bit_Map.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="47">
   <si>
     <t>State ID</t>
   </si>
@@ -63,6 +63,108 @@
   </si>
   <si>
     <t>bne</t>
+  </si>
+  <si>
+    <t>jr</t>
+  </si>
+  <si>
+    <t>Control Signal</t>
+  </si>
+  <si>
+    <t>branch</t>
+  </si>
+  <si>
+    <t>PCwrt</t>
+  </si>
+  <si>
+    <t>IRwrt</t>
+  </si>
+  <si>
+    <t>memOWrt</t>
+  </si>
+  <si>
+    <t>Awrt</t>
+  </si>
+  <si>
+    <t>Bwrt</t>
+  </si>
+  <si>
+    <t>ALUwrt</t>
+  </si>
+  <si>
+    <t>regWrt</t>
+  </si>
+  <si>
+    <t>memWrt</t>
+  </si>
+  <si>
+    <t>wAdrs</t>
+  </si>
+  <si>
+    <t>wDat[1:0]</t>
+  </si>
+  <si>
+    <t>memAdrsSlct</t>
+  </si>
+  <si>
+    <t>immSlct</t>
+  </si>
+  <si>
+    <t>BNEoBEQ</t>
+  </si>
+  <si>
+    <t>jump[1:0]</t>
+  </si>
+  <si>
+    <t>imOrR[1:0]</t>
+  </si>
+  <si>
+    <t>00 default, 01 if jumping, 10 if jumping to register</t>
+  </si>
+  <si>
+    <t>high if writing to pc</t>
+  </si>
+  <si>
+    <t>high if writing to IR</t>
+  </si>
+  <si>
+    <t>high if writing to MemOWrt</t>
+  </si>
+  <si>
+    <t>high if writing to AiA</t>
+  </si>
+  <si>
+    <t>high if writing to AiB</t>
+  </si>
+  <si>
+    <t>high if writing to ALUout</t>
+  </si>
+  <si>
+    <t>high if writing to Reg. File</t>
+  </si>
+  <si>
+    <t>high if writing to Mem File</t>
+  </si>
+  <si>
+    <t>controls mux into wDest, default is $m, high if address from IR</t>
+  </si>
+  <si>
+    <t>controls mux into wData, 00 if from memO, 01 if from ALUout, 10 if from AiA, 11 if from Sign Ext.</t>
+  </si>
+  <si>
+    <t>controls mux into adrs of Mem, default pc, high if ALUout</t>
+  </si>
+  <si>
+    <t>controls mux into Sign Ext., default is 12 bit immediate, high is 10 bit immediate</t>
+  </si>
+  <si>
+    <t>controls mux out of isZero from ALU, default is isZero (used for BEQ), high is ~(isZero)  (used for BNE)</t>
+  </si>
+  <si>
+    <t>controls mux into AiB, default r2out from Reg File, 01 from Sign Ext., 10 from PC+1 (for JR), 11 empty (currently)</t>
+  </si>
+  <si>
+    <t>controls mux into pc adder, default is PC+1, high is Sign Ext. (for branching)</t>
   </si>
 </sst>
 </file>
@@ -385,10 +487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -396,9 +498,11 @@
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="9.140625" style="2"/>
     <col min="3" max="3" width="49.7109375" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="101.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -408,8 +512,14 @@
       <c r="C1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -420,8 +530,14 @@
       <c r="C2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -432,8 +548,14 @@
       <c r="C3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>10</v>
       </c>
@@ -444,8 +566,14 @@
       <c r="C4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>11</v>
       </c>
@@ -456,8 +584,14 @@
       <c r="C5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>100</v>
       </c>
@@ -468,8 +602,14 @@
       <c r="C6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>101</v>
       </c>
@@ -480,8 +620,14 @@
       <c r="C7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>110</v>
       </c>
@@ -492,8 +638,14 @@
       <c r="C8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>111</v>
       </c>
@@ -504,8 +656,14 @@
       <c r="C9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>1000</v>
       </c>
@@ -516,8 +674,14 @@
       <c r="C10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>1001</v>
       </c>
@@ -528,8 +692,14 @@
       <c r="C11" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>1010</v>
       </c>
@@ -540,8 +710,14 @@
       <c r="C12" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>1011</v>
       </c>
@@ -552,8 +728,14 @@
       <c r="C13" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>1100</v>
       </c>
@@ -564,8 +746,14 @@
       <c r="C14" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>1101</v>
       </c>
@@ -576,8 +764,14 @@
       <c r="C15" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>1110</v>
       </c>
@@ -588,8 +782,14 @@
       <c r="C16" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>27</v>
+      </c>
+      <c r="F16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>1111</v>
       </c>
@@ -600,8 +800,14 @@
       <c r="C17" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>28</v>
+      </c>
+      <c r="F17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>10000</v>
       </c>
@@ -613,7 +819,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>10001</v>
       </c>
@@ -625,7 +831,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>10010</v>
       </c>
@@ -637,7 +843,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>10011</v>
       </c>
@@ -649,7 +855,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>10100</v>
       </c>
@@ -661,7 +867,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>10101</v>
       </c>
@@ -673,7 +879,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>10110</v>
       </c>
@@ -681,8 +887,11 @@
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>10111</v>
       </c>
@@ -690,8 +899,11 @@
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>11000</v>
       </c>
@@ -699,8 +911,11 @@
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>11001</v>
       </c>
@@ -709,7 +924,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>11010</v>
       </c>
@@ -718,7 +933,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>11011</v>
       </c>
@@ -727,7 +942,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>11100</v>
       </c>
@@ -736,7 +951,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>11101</v>
       </c>
@@ -745,7 +960,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>11110</v>
       </c>

</xml_diff>